<commit_message>
add supporting html files - minor changes to resume
</commit_message>
<xml_diff>
--- a/resume_data.xlsx
+++ b/resume_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mattl\OneDrive\Documents\Personal\rProjects\cv_leary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mattl\OneDrive\Documents\Personal\rProjects\resume\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B03F08F7-D2B9-4AAE-8C73-13AB32B4F923}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C99E2D57-1462-4F6A-A33D-94B04F6759CA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="positions" sheetId="1" r:id="rId1"/>
@@ -228,15 +228,9 @@
     <t>Regularly uses R, Python, Git, SQL , and sources data from databases, XMLs, API calls, etc.</t>
   </si>
   <si>
-    <t>Data scientist on an agile sprint team supporting the growth of insurance product lines by building applications that help prioritize and monitor incoming business</t>
-  </si>
-  <si>
     <t>Communicates technical matters, such as model selection and maintenance, to business owners and works to advance the analytics capabilities within the company</t>
   </si>
   <si>
-    <t>Develops, maintains, and deploys machine learning models to end users and helps to automate processes via command line tools and scripts</t>
-  </si>
-  <si>
     <t>description_5</t>
   </si>
   <si>
@@ -246,7 +240,13 @@
     <t>Print journalist and public affairs manager for a 4,000-person organization, supervised three direct reports, advised executive staff, and  deployed twice to Afghanistan</t>
   </si>
   <si>
-    <t>M.S., Decision Analytics        |       Master of Business Administration</t>
+    <t>M.S., Decision Analytics        &amp;       Master of Business Administration</t>
+  </si>
+  <si>
+    <t>Data scientist on an agile sprint team that builds, deploys, and maintains production applications that help prioritize and monitor incoming business</t>
+  </si>
+  <si>
+    <t>Develops, maintains, and deploys machine learning models to end users and conducts ad hoc analysis that help drive decision making</t>
   </si>
 </sst>
 </file>
@@ -1105,7 +1105,7 @@
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1150,7 +1150,7 @@
         <v>45</v>
       </c>
       <c r="L1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="M1" t="s">
         <v>64</v>
@@ -1164,7 +1164,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
@@ -1250,19 +1250,19 @@
         <v>17</v>
       </c>
       <c r="H6" t="s">
+        <v>73</v>
+      </c>
+      <c r="I6" t="s">
+        <v>74</v>
+      </c>
+      <c r="J6" t="s">
         <v>68</v>
-      </c>
-      <c r="I6" t="s">
-        <v>70</v>
-      </c>
-      <c r="J6" t="s">
-        <v>69</v>
       </c>
       <c r="K6" t="s">
         <v>67</v>
       </c>
       <c r="L6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
@@ -1393,7 +1393,7 @@
         <v>2010</v>
       </c>
       <c r="H10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I10" t="s">
         <v>44</v>

</xml_diff>

<commit_message>
fixed some color issues involving the bullets, fixed a delete item from data file
</commit_message>
<xml_diff>
--- a/resume_data.xlsx
+++ b/resume_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mattl\OneDrive\Documents\Personal\rProjects\resume\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C99E2D57-1462-4F6A-A33D-94B04F6759CA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB05E40-9C1E-474D-80A8-612CD6A61BC0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -240,13 +240,13 @@
     <t>Print journalist and public affairs manager for a 4,000-person organization, supervised three direct reports, advised executive staff, and  deployed twice to Afghanistan</t>
   </si>
   <si>
-    <t>M.S., Decision Analytics        &amp;       Master of Business Administration</t>
-  </si>
-  <si>
     <t>Data scientist on an agile sprint team that builds, deploys, and maintains production applications that help prioritize and monitor incoming business</t>
   </si>
   <si>
     <t>Develops, maintains, and deploys machine learning models to end users and conducts ad hoc analysis that help drive decision making</t>
+  </si>
+  <si>
+    <t>M.S., Decision Analytics   |   M.B.A.</t>
   </si>
 </sst>
 </file>
@@ -1105,7 +1105,7 @@
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1164,7 +1164,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
@@ -1250,10 +1250,10 @@
         <v>17</v>
       </c>
       <c r="H6" t="s">
+        <v>72</v>
+      </c>
+      <c r="I6" t="s">
         <v>73</v>
-      </c>
-      <c r="I6" t="s">
-        <v>74</v>
       </c>
       <c r="J6" t="s">
         <v>68</v>

</xml_diff>